<commit_message>
Atualizando data/season_2025/next_games/next_games.xlsx via script
</commit_message>
<xml_diff>
--- a/data/season_2025/next_games/next_games.xlsx
+++ b/data/season_2025/next_games/next_games.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V34"/>
+  <dimension ref="A1:V47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -558,92 +558,76 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Liga Portugal - PRT PL</t>
+          <t>Pro League - BEL FDA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Vitória Guimarães vs Sporting CP</t>
+          <t>Genk vs Club Brugge</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-12-23 20:45:00</t>
+          <t>2025-12-26 12:30:00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>6.25</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>4.33</t>
+          <t>3.50</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1.45</t>
+          <t>2.15</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>7.29</t>
+          <t>3.14</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>4.62</t>
+          <t>3.67</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1.46</t>
+          <t>2.23</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>1.75</t>
+          <t>2.37</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2.00</t>
+          <t>1.53</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>1.78</t>
+          <t>2.46</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2.09</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>1.92</t>
-        </is>
-      </c>
+          <t>1.57</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>1.92</t>
-        </is>
-      </c>
+      <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>1.93</t>
-        </is>
-      </c>
+      <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>1.95</t>
-        </is>
-      </c>
+      <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
       <c r="V2" s="2" t="inlineStr">
         <is>
@@ -659,163 +643,155 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Al-Fayha vs Al Hazm</t>
+          <t>Al Fateh vs Al Ahli</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-12-25 14:50:00</t>
+          <t>2025-12-26 13:05:00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1.80</t>
+          <t>4.50</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>3.40</t>
+          <t>3.80</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>4.00</t>
+          <t>1.57</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>1.83</t>
+          <t>4.52</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>3.59</t>
+          <t>4.47</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>4.07</t>
+          <t>1.62</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>1.83</t>
+          <t>2.37</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>1.83</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>1.88</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>1.88</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>2.02</t>
-        </is>
-      </c>
+          <t>1.53</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>1.77</t>
-        </is>
-      </c>
+      <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>2.01</t>
-        </is>
-      </c>
+      <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>1.79</t>
-        </is>
-      </c>
+      <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Pro League - SAU PL</t>
+          <t>Pro League - BEL FDA</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>NEOM SC vs Al Najma</t>
+          <t>Cercle Brugge vs Union Saint-Gilloise</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-12-25 17:30:00</t>
+          <t>2025-12-26 15:00:00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.40</t>
+          <t>3.70</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>4.20</t>
+          <t>3.50</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>6.50</t>
+          <t>1.85</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>1.42</t>
+          <t>3.92</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>4.67</t>
+          <t>3.69</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>6.42</t>
+          <t>1.94</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>1.83</t>
+          <t>2.05</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>1.83</t>
+          <t>1.70</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>1.92</t>
+          <t>2.15</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>1.83</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr"/>
+          <t>1.73</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>1.80</t>
+        </is>
+      </c>
       <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
       <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>1.85</t>
+        </is>
+      </c>
       <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>2.02</t>
+        </is>
+      </c>
       <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
     </row>
@@ -827,12 +803,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Al Riyadh vs Al Ettifaq</t>
+          <t>Al Kholood vs Al Taawoun</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-12-25 17:30:00</t>
+          <t>2025-12-26 15:00:00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -847,57 +823,65 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2.20</t>
+          <t>2.10</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2.94</t>
+          <t>3.18</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>3.40</t>
+          <t>3.58</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2.32</t>
+          <t>2.16</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>2.00</t>
+          <t>2.10</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>1.72</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
+          <t>1.66</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>2.18</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>1.67</t>
+        </is>
+      </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>1.95</t>
+          <t>1.80</t>
         </is>
       </c>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr">
         <is>
-          <t>1.85</t>
+          <t>2.00</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr">
         <is>
-          <t>1.90</t>
+          <t>1.83</t>
         </is>
       </c>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr">
         <is>
-          <t>1.87</t>
+          <t>1.99</t>
         </is>
       </c>
       <c r="U5" t="inlineStr"/>
@@ -911,63 +895,87 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Genk vs Club Brugge</t>
+          <t>Standard Liège vs Sint-Truiden</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-12-26 12:30:00</t>
+          <t>2025-12-26 17:30:00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2.90</t>
+          <t>2.80</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>3.50</t>
+          <t>3.30</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2.15</t>
+          <t>2.30</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2.99</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>3.55</t>
+          <t>3.38</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2.30</t>
+          <t>2.44</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>2.25</t>
+          <t>2.05</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>1.57</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
+          <t>1.70</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>2.23</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>1.68</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>1.90</t>
+        </is>
+      </c>
       <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>1.90</t>
+        </is>
+      </c>
       <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>1.91</t>
+        </is>
+      </c>
       <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>1.95</t>
+        </is>
+      </c>
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
     </row>
@@ -979,64 +987,88 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Al Fateh vs Al Ahli</t>
+          <t>Al Hilal vs Al Khaleej</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-12-26 13:05:00</t>
+          <t>2025-12-26 17:30:00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>4.75</t>
+          <t>1.20</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>3.90</t>
+          <t>6.00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>1.50</t>
+          <t>9.50</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>5.05</t>
+          <t>1.15</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>4.63</t>
+          <t>8.42</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1.51</t>
+          <t>12.55</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>2.25</t>
+          <t>2.10</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>1.57</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
+          <t>1.66</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>2.16</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>1.67</t>
+        </is>
+      </c>
       <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
       <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>1.80</t>
+        </is>
+      </c>
       <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>1.80</t>
+        </is>
+      </c>
       <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr"/>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
       <c r="V7" t="inlineStr"/>
     </row>
     <row r="8">
@@ -1047,17 +1079,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Cercle Brugge vs Union Saint-Gilloise</t>
+          <t>Anderlecht vs Sporting Charleroi</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-12-26 15:00:00</t>
+          <t>2025-12-26 19:45:00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>3.60</t>
+          <t>1.75</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1067,65 +1099,65 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>1.90</t>
+          <t>4.33</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>3.90</t>
+          <t>1.77</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>3.66</t>
+          <t>3.65</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>1.91</t>
+          <t>4.92</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>2.05</t>
+          <t>1.80</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>1.70</t>
+          <t>1.95</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>2.13</t>
+          <t>1.92</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>1.72</t>
+          <t>1.92</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>2.00</t>
+          <t>2.02</t>
         </is>
       </c>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr">
         <is>
-          <t>1.80</t>
+          <t>1.77</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr">
         <is>
-          <t>1.83</t>
+          <t>2.06</t>
         </is>
       </c>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr">
         <is>
-          <t>2.01</t>
+          <t>1.81</t>
         </is>
       </c>
       <c r="U8" t="inlineStr"/>
@@ -1134,277 +1166,229 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Pro League - SAU PL</t>
+          <t>Premier League - UK PL</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Al Kholood vs Al Taawoun</t>
+          <t>Manchester United vs Newcastle United</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-12-26 15:00:00</t>
+          <t>2025-12-26 20:00:00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>3.00</t>
+          <t>2.50</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>3.20</t>
+          <t>3.60</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2.10</t>
+          <t>2.62</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>3.16</t>
+          <t>2.57</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>3.46</t>
+          <t>3.65</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>2.17</t>
+          <t>2.70</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>2.00</t>
+          <t>2.37</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>1.72</t>
+          <t>1.53</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>2.15</t>
+          <t>2.60</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>1.67</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>1.85</t>
-        </is>
-      </c>
+          <t>1.53</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>1.95</t>
-        </is>
-      </c>
+      <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>1.84</t>
-        </is>
-      </c>
+      <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>1.93</t>
-        </is>
-      </c>
+      <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Pro League - BEL FDA</t>
+          <t>Serie A - ITA SA</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Standard Liège vs Sint-Truiden</t>
+          <t>Parma vs Fiorentina</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-12-26 17:30:00</t>
+          <t>2025-12-27 11:30:00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2.70</t>
+          <t>3.50</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>3.30</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2.37</t>
+          <t>2.25</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2.84</t>
+          <t>3.54</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>3.29</t>
+          <t>3.09</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>2.55</t>
+          <t>2.34</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>2.05</t>
+          <t>1.90</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>1.70</t>
+          <t>1.90</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>2.21</t>
+          <t>1.95</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>1.67</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
           <t>1.90</t>
         </is>
       </c>
+      <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>1.90</t>
-        </is>
-      </c>
+      <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>1.90</t>
-        </is>
-      </c>
+      <c r="R10" t="inlineStr"/>
       <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>1.92</t>
-        </is>
-      </c>
+      <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Pro League - SAU PL</t>
+          <t>Premier League - UK PL</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Al Hilal vs Al Khaleej</t>
+          <t>Nottingham Forest vs Manchester City</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-12-26 17:30:00</t>
+          <t>2025-12-27 12:30:00</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.20</t>
+          <t>5.00</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>5.75</t>
+          <t>4.33</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>9.50</t>
+          <t>1.57</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>1.19</t>
+          <t>5.34</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>7.34</t>
+          <t>4.66</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>9.84</t>
+          <t>1.57</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>1.90</t>
+          <t>2.10</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>1.80</t>
+          <t>1.66</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2.03</t>
+          <t>2.26</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>1.73</t>
+          <t>1.68</t>
         </is>
       </c>
       <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>1.85</t>
-        </is>
-      </c>
+      <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>1.95</t>
-        </is>
-      </c>
+      <c r="Q11" t="inlineStr"/>
       <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>1.87</t>
-        </is>
-      </c>
+      <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr">
-        <is>
-          <t>1.89</t>
-        </is>
-      </c>
+      <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr"/>
     </row>
     <row r="12">
@@ -1415,85 +1399,85 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Anderlecht vs Sporting Charleroi</t>
+          <t>Antwerp vs Zulte-Waregem</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-12-26 19:45:00</t>
+          <t>2025-12-27 12:30:00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.75</t>
+          <t>1.95</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
+          <t>3.40</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
           <t>3.50</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>4.33</t>
-        </is>
-      </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>1.76</t>
+          <t>2.02</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>3.61</t>
+          <t>3.66</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>4.81</t>
+          <t>3.54</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>1.90</t>
+          <t>2.05</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>1.90</t>
+          <t>1.70</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>1.90</t>
+          <t>2.12</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>1.90</t>
+          <t>1.72</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>2.02</t>
+          <t>1.85</t>
         </is>
       </c>
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr">
         <is>
-          <t>1.77</t>
+          <t>1.95</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr"/>
       <c r="R12" t="inlineStr">
         <is>
-          <t>2.04</t>
+          <t>1.87</t>
         </is>
       </c>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr">
         <is>
-          <t>1.80</t>
+          <t>1.96</t>
         </is>
       </c>
       <c r="U12" t="inlineStr"/>
@@ -1502,69 +1486,61 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Premier League - UK PL</t>
+          <t>Pro League - SAU PL</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Manchester United vs Newcastle United</t>
+          <t>Al-Qadsiah vs Damac FC</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-12-26 20:00:00</t>
+          <t>2025-12-27 13:00:00</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2.50</t>
+          <t>1.30</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>3.60</t>
+          <t>4.75</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2.60</t>
+          <t>8.50</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2.59</t>
+          <t>1.29</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>3.73</t>
+          <t>5.61</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>2.64</t>
+          <t>8.04</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>2.37</t>
+          <t>1.83</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>1.53</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>2.61</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>1.52</t>
-        </is>
-      </c>
+          <t>1.83</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr"/>
@@ -1583,62 +1559,62 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Parma vs Fiorentina</t>
+          <t>Lecce vs Como</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-12-27 11:30:00</t>
+          <t>2025-12-27 14:00:00</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>3.50</t>
+          <t>4.75</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>3.00</t>
+          <t>3.30</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2.25</t>
+          <t>1.80</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>3.53</t>
+          <t>4.91</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>3.11</t>
+          <t>3.43</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>2.33</t>
+          <t>1.85</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>1.90</t>
+          <t>1.70</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>1.90</t>
+          <t>2.05</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>1.96</t>
+          <t>1.76</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>1.89</t>
+          <t>2.12</t>
         </is>
       </c>
       <c r="N14" t="inlineStr"/>
@@ -1654,67 +1630,67 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Premier League - UK PL</t>
+          <t>Serie A - ITA SA</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Nottingham Forest vs Manchester City</t>
+          <t>Torino vs Cagliari</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-12-27 12:30:00</t>
+          <t>2025-12-27 14:00:00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>5.25</t>
+          <t>1.90</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
+          <t>3.20</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
           <t>4.20</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>1.57</t>
-        </is>
-      </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>5.13</t>
+          <t>2.01</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>4.42</t>
+          <t>3.29</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>1.62</t>
+          <t>4.29</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>2.05</t>
+          <t>1.80</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>1.70</t>
+          <t>1.95</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>2.23</t>
+          <t>1.89</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>1.69</t>
+          <t>1.96</t>
         </is>
       </c>
       <c r="N15" t="inlineStr"/>
@@ -1730,131 +1706,131 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Pro League - BEL FDA</t>
+          <t>Pro League - SAU PL</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Antwerp vs Zulte-Waregem</t>
+          <t>Al Nassr vs Al Akhdoud</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-12-27 12:30:00</t>
+          <t>2025-12-27 14:50:00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.95</t>
+          <t>1.10</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>3.40</t>
+          <t>9.00</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>3.50</t>
+          <t>19.00</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>1.99</t>
+          <t>1.07</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>3.82</t>
+          <t>13.05</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>3.49</t>
+          <t>18.25</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>2.05</t>
+          <t>1.61</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>1.70</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>1.82</t>
-        </is>
-      </c>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr">
-        <is>
-          <t>1.97</t>
-        </is>
-      </c>
-      <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="inlineStr">
-        <is>
-          <t>1.85</t>
-        </is>
-      </c>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>1.60</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>2.24</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>1.80</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr"/>
       <c r="S16" t="inlineStr"/>
-      <c r="T16" t="inlineStr">
-        <is>
-          <t>1.98</t>
-        </is>
-      </c>
+      <c r="T16" t="inlineStr"/>
       <c r="U16" t="inlineStr"/>
       <c r="V16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Pro League - SAU PL</t>
+          <t>Premier League - UK PL</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Al-Qadsiah vs Damac FC</t>
+          <t>Arsenal vs Brighton &amp; Hove Albion</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-12-27 13:00:00</t>
+          <t>2025-12-27 15:00:00</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.36</t>
+          <t>1.38</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>4.33</t>
+          <t>5.00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>8.00</t>
+          <t>7.50</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>1.34</t>
+          <t>1.39</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>5.09</t>
+          <t>5.06</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>7.36</t>
+          <t>8.22</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1864,11 +1840,19 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>1.90</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
+          <t>1.95</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>1.91</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>1.94</t>
+        </is>
+      </c>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr"/>
@@ -1882,67 +1866,67 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Serie A - ITA SA</t>
+          <t>Premier League - UK PL</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Lecce vs Como</t>
+          <t>Brentford vs AFC Bournemouth</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-12-27 14:00:00</t>
+          <t>2025-12-27 15:00:00</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>4.75</t>
+          <t>2.25</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>3.30</t>
+          <t>3.60</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>1.80</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>4.89</t>
+          <t>2.31</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>3.52</t>
+          <t>3.65</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1.83</t>
+          <t>3.07</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>1.70</t>
+          <t>2.25</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2.05</t>
+          <t>1.57</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>1.76</t>
+          <t>2.44</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>2.12</t>
+          <t>1.59</t>
         </is>
       </c>
       <c r="N18" t="inlineStr"/>
@@ -1958,47 +1942,47 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Serie A - ITA SA</t>
+          <t>Premier League - UK PL</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Torino vs Cagliari</t>
+          <t>Burnley vs Everton</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-12-27 14:00:00</t>
+          <t>2025-12-27 15:00:00</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.90</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>3.30</t>
+          <t>3.40</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>4.10</t>
+          <t>2.00</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>1.98</t>
+          <t>4.13</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>3.39</t>
+          <t>3.35</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>4.25</t>
+          <t>2.03</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -2034,73 +2018,73 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Pro League - SAU PL</t>
+          <t>Premier League - UK PL</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Al Nassr vs Al Akhdoud</t>
+          <t>Liverpool vs Wolverhampton Wanderers</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-12-27 14:50:00</t>
+          <t>2025-12-27 15:00:00</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.11</t>
+          <t>1.25</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>8.50</t>
+          <t>7.00</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>19.00</t>
+          <t>10.00</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>1.07</t>
+          <t>1.23</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>12.82</t>
+          <t>7.00</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>17.76</t>
+          <t>11.66</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>1.61</t>
+          <t>1.75</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2.20</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr"/>
+          <t>2.00</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>1.78</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>2.08</t>
+        </is>
+      </c>
       <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>2.00</t>
-        </is>
-      </c>
+      <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr"/>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>1.80</t>
-        </is>
-      </c>
+      <c r="Q20" t="inlineStr"/>
       <c r="R20" t="inlineStr"/>
       <c r="S20" t="inlineStr"/>
       <c r="T20" t="inlineStr"/>
@@ -2115,7 +2099,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Arsenal vs Brighton &amp; Hove Albion</t>
+          <t>West Ham United vs Fulham</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -2125,73 +2109,89 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.40</t>
+          <t>2.62</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>4.50</t>
+          <t>3.40</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>7.50</t>
+          <t>2.60</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>1.42</t>
+          <t>2.69</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>4.89</t>
+          <t>3.48</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>7.76</t>
+          <t>2.68</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>1.90</t>
+          <t>2.20</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>1.90</t>
+          <t>1.61</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>1.92</t>
+          <t>2.35</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>1.92</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr"/>
+          <t>1.63</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>2.02</t>
+        </is>
+      </c>
       <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr"/>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>1.82</t>
+        </is>
+      </c>
       <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="inlineStr"/>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>1.81</t>
+        </is>
+      </c>
       <c r="S21" t="inlineStr"/>
-      <c r="T21" t="inlineStr"/>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>2.03</t>
+        </is>
+      </c>
       <c r="U21" t="inlineStr"/>
       <c r="V21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Premier League - UK PL</t>
+          <t>Pro League - BEL FDA</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Brentford vs AFC Bournemouth</t>
+          <t>La Louvière vs OH Leuven</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2201,27 +2201,27 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2.25</t>
+          <t>2.40</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>3.60</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>3.00</t>
+          <t>3.10</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2.31</t>
+          <t>2.55</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>3.66</t>
+          <t>3.03</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -2231,24 +2231,16 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>2.25</t>
+          <t>1.80</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>1.57</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>2.42</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>1.60</t>
-        </is>
-      </c>
+          <t>1.95</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="inlineStr"/>
@@ -2262,67 +2254,67 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Premier League - UK PL</t>
+          <t>Serie A - ITA SA</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Burnley vs Everton</t>
+          <t>Udinese vs Lazio</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-12-27 15:00:00</t>
+          <t>2025-12-27 17:00:00</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>4.10</t>
+          <t>3.10</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>3.40</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
+          <t>2.45</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>3.16</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>3.07</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>2.55</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>1.80</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
           <t>1.95</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>4.12</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>3.36</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>2.03</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>1.80</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>1.95</t>
-        </is>
-      </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>1.86</t>
+          <t>1.91</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>1.99</t>
+          <t>1.94</t>
         </is>
       </c>
       <c r="N23" t="inlineStr"/>
@@ -2338,76 +2330,84 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Premier League - UK PL</t>
+          <t>Pro League - BEL FDA</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Liverpool vs Wolverhampton Wanderers</t>
+          <t>Mechelen vs Dender</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-12-27 15:00:00</t>
+          <t>2025-12-27 17:15:00</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1.22</t>
+          <t>2.10</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>6.50</t>
+          <t>3.40</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>10.00</t>
+          <t>3.20</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>1.23</t>
+          <t>2.16</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>7.03</t>
+          <t>3.54</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>11.72</t>
+          <t>3.29</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>1.80</t>
+          <t>2.10</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>1.95</t>
+          <t>1.66</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>1.81</t>
+          <t>2.24</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>2.04</t>
+          <t>1.65</t>
         </is>
       </c>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr"/>
       <c r="Q24" t="inlineStr"/>
-      <c r="R24" t="inlineStr"/>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>1.81</t>
+        </is>
+      </c>
       <c r="S24" t="inlineStr"/>
-      <c r="T24" t="inlineStr"/>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
       <c r="U24" t="inlineStr"/>
       <c r="V24" t="inlineStr"/>
     </row>
@@ -2419,128 +2419,140 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>West Ham United vs Fulham</t>
+          <t>Chelsea vs Aston Villa</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-12-27 15:00:00</t>
+          <t>2025-12-27 17:30:00</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2.62</t>
+          <t>1.83</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>3.40</t>
+          <t>3.90</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2.62</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2.70</t>
+          <t>1.85</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>3.47</t>
+          <t>3.98</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2.67</t>
+          <t>4.10</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>2.20</t>
+          <t>2.10</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>1.61</t>
+          <t>1.66</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2.33</t>
+          <t>2.31</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>1.64</t>
-        </is>
-      </c>
-      <c r="N25" t="inlineStr">
-        <is>
-          <t>2.02</t>
-        </is>
-      </c>
+          <t>1.65</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr"/>
       <c r="O25" t="inlineStr"/>
-      <c r="P25" t="inlineStr">
-        <is>
-          <t>1.82</t>
-        </is>
-      </c>
+      <c r="P25" t="inlineStr"/>
       <c r="Q25" t="inlineStr"/>
-      <c r="R25" t="inlineStr">
-        <is>
-          <t>1.81</t>
-        </is>
-      </c>
+      <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr"/>
-      <c r="T25" t="inlineStr">
-        <is>
-          <t>2.03</t>
-        </is>
-      </c>
+      <c r="T25" t="inlineStr"/>
       <c r="U25" t="inlineStr"/>
       <c r="V25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Pro League - BEL FDA</t>
+          <t>Pro League - SAU PL</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>La Louvière vs OH Leuven</t>
+          <t>Al Ittihad vs Al Shabab</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-12-27 15:00:00</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
+          <t>2025-12-27 17:30:00</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>1.55</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>4.10</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>4.75</t>
+        </is>
+      </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2.55</t>
+          <t>1.56</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>3.03</t>
+          <t>4.30</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>3.05</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="inlineStr"/>
+          <t>4.98</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>1.61</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>2.21</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>1.63</t>
+        </is>
+      </c>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="inlineStr"/>
@@ -2554,47 +2566,47 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Serie A - ITA SA</t>
+          <t>Liga Portugal - PRT PL</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Udinese vs Lazio</t>
+          <t>Famalicão vs Estrela Amadora</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-12-27 17:00:00</t>
+          <t>2025-12-27 18:00:00</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>3.10</t>
+          <t>1.57</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>3.00</t>
+          <t>3.70</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2.45</t>
+          <t>6.00</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>3.14</t>
+          <t>1.59</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>3.08</t>
+          <t>3.95</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2.56</t>
+          <t>5.82</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2607,69 +2619,129 @@
           <t>1.95</t>
         </is>
       </c>
-      <c r="L27" t="inlineStr"/>
-      <c r="M27" t="inlineStr"/>
-      <c r="N27" t="inlineStr"/>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>1.82</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>1.97</t>
+        </is>
+      </c>
       <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr"/>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>1.87</t>
+        </is>
+      </c>
       <c r="Q27" t="inlineStr"/>
-      <c r="R27" t="inlineStr"/>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
       <c r="S27" t="inlineStr"/>
-      <c r="T27" t="inlineStr"/>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>1.84</t>
+        </is>
+      </c>
       <c r="U27" t="inlineStr"/>
       <c r="V27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Pro League - BEL FDA</t>
+          <t>Serie A - ITA SA</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Mechelen vs Dender</t>
+          <t>Pisa vs Juventus</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-12-27 17:15:00</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
+          <t>2025-12-27 19:45:00</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>7.50</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>4.50</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>1.40</t>
+        </is>
+      </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2.15</t>
+          <t>7.07</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>3.58</t>
+          <t>4.61</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>3.26</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr"/>
-      <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr"/>
-      <c r="M28" t="inlineStr"/>
-      <c r="N28" t="inlineStr"/>
+          <t>1.47</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>1.66</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>2.10</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>1.72</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>2.18</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>1.97</t>
+        </is>
+      </c>
       <c r="O28" t="inlineStr"/>
-      <c r="P28" t="inlineStr"/>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>1.87</t>
+        </is>
+      </c>
       <c r="Q28" t="inlineStr"/>
       <c r="R28" t="inlineStr">
         <is>
-          <t>1.81</t>
+          <t>2.00</t>
         </is>
       </c>
       <c r="S28" t="inlineStr"/>
       <c r="T28" t="inlineStr">
         <is>
-          <t>2.00</t>
+          <t>1.89</t>
         </is>
       </c>
       <c r="U28" t="inlineStr"/>
@@ -2678,67 +2750,67 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Premier League - UK PL</t>
+          <t>Pro League - BEL FDA</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Chelsea vs Aston Villa</t>
+          <t>Gent vs Westerlo</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-12-27 17:30:00</t>
+          <t>2025-12-27 19:45:00</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.83</t>
+          <t>2.25</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>3.80</t>
+          <t>3.60</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>3.90</t>
+          <t>2.80</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>1.87</t>
+          <t>2.32</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>3.91</t>
+          <t>3.79</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>4.07</t>
+          <t>2.81</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>2.10</t>
+          <t>2.50</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>1.66</t>
+          <t>1.50</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2.24</t>
+          <t>2.63</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>1.69</t>
+          <t>1.49</t>
         </is>
       </c>
       <c r="N29" t="inlineStr"/>
@@ -2754,61 +2826,69 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Pro League - SAU PL</t>
+          <t>Liga Portugal - PRT PL</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Al Ittihad vs Al Shabab</t>
+          <t>Estoril vs Alverca</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2025-12-27 17:30:00</t>
+          <t>2025-12-27 20:30:00</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.48</t>
+          <t>2.20</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>4.33</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>5.00</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>1.49</t>
+          <t>2.24</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>4.56</t>
+          <t>3.46</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>5.43</t>
+          <t>3.17</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>2.20</t>
+          <t>1.95</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>1.61</t>
-        </is>
-      </c>
-      <c r="L30" t="inlineStr"/>
-      <c r="M30" t="inlineStr"/>
+          <t>1.80</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>1.95</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>1.85</t>
+        </is>
+      </c>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr"/>
@@ -2822,67 +2902,67 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Liga Portugal - PRT PL</t>
+          <t>Liga Portugal 2 - PRT SL</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Famalicão vs Estrela Amadora</t>
+          <t>Academico Viseu vs Benfica II</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-12-27 18:00:00</t>
+          <t>2025-12-28 11:00:00</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.55</t>
+          <t>1.66</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>3.80</t>
+          <t>3.40</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>6.00</t>
+          <t>4.33</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>1.55</t>
+          <t>1.72</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>4.03</t>
+          <t>3.73</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>6.12</t>
+          <t>4.70</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>1.80</t>
+          <t>1.83</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>1.95</t>
+          <t>1.83</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>1.79</t>
+          <t>1.94</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>2.02</t>
+          <t>1.84</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
@@ -2893,19 +2973,19 @@
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="inlineStr">
         <is>
-          <t>1.87</t>
+          <t>1.82</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr"/>
       <c r="R31" t="inlineStr">
         <is>
-          <t>1.97</t>
+          <t>1.96</t>
         </is>
       </c>
       <c r="S31" t="inlineStr"/>
       <c r="T31" t="inlineStr">
         <is>
-          <t>1.86</t>
+          <t>1.85</t>
         </is>
       </c>
       <c r="U31" t="inlineStr"/>
@@ -2919,42 +2999,42 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Pisa vs Juventus</t>
+          <t>Milan vs Hellas Verona</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-12-27 19:45:00</t>
+          <t>2025-12-28 11:30:00</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>7.50</t>
+          <t>1.38</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>4.50</t>
+          <t>4.75</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>1.40</t>
+          <t>8.50</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>7.06</t>
+          <t>1.38</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>4.64</t>
+          <t>4.98</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>1.47</t>
+          <t>8.82</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -2969,35 +3049,35 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>1.74</t>
+          <t>1.78</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>2.17</t>
+          <t>2.11</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>1.97</t>
+          <t>1.85</t>
         </is>
       </c>
       <c r="O32" t="inlineStr"/>
       <c r="P32" t="inlineStr">
         <is>
-          <t>1.87</t>
+          <t>2.00</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr"/>
       <c r="R32" t="inlineStr">
         <is>
-          <t>1.98</t>
+          <t>1.86</t>
         </is>
       </c>
       <c r="S32" t="inlineStr"/>
       <c r="T32" t="inlineStr">
         <is>
-          <t>1.90</t>
+          <t>2.03</t>
         </is>
       </c>
       <c r="U32" t="inlineStr"/>
@@ -3006,135 +3086,159 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Pro League - BEL FDA</t>
+          <t>Serie A - ITA SA</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Gent vs Westerlo</t>
+          <t>Cremonese vs Napoli</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2025-12-27 19:45:00</t>
+          <t>2025-12-28 14:00:00</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2.25</t>
+          <t>6.25</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>3.60</t>
+          <t>3.90</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2.80</t>
+          <t>1.55</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2.31</t>
+          <t>6.30</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>3.81</t>
+          <t>4.14</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>2.83</t>
+          <t>1.57</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>2.50</t>
+          <t>1.66</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>1.50</t>
-        </is>
-      </c>
-      <c r="L33" t="inlineStr"/>
-      <c r="M33" t="inlineStr"/>
-      <c r="N33" t="inlineStr"/>
+          <t>2.10</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>1.73</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>2.17</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>1.82</t>
+        </is>
+      </c>
       <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr"/>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>2.02</t>
+        </is>
+      </c>
       <c r="Q33" t="inlineStr"/>
-      <c r="R33" t="inlineStr"/>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>2.08</t>
+        </is>
+      </c>
       <c r="S33" t="inlineStr"/>
-      <c r="T33" t="inlineStr"/>
+      <c r="T33" t="inlineStr">
+        <is>
+          <t>1.81</t>
+        </is>
+      </c>
       <c r="U33" t="inlineStr"/>
       <c r="V33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Liga Portugal - PRT PL</t>
+          <t>Premier League - UK PL</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Estoril vs Alverca</t>
+          <t>Sunderland vs Leeds United</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-12-27 20:30:00</t>
+          <t>2025-12-28 14:00:00</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2.20</t>
+          <t>2.50</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>3.25</t>
+          <t>3.10</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>3.25</t>
+          <t>2.87</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2.28</t>
+          <t>2.63</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>3.45</t>
+          <t>3.31</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>3.11</t>
+          <t>2.85</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>1.95</t>
+          <t>1.90</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>1.80</t>
+          <t>1.90</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>1.95</t>
+          <t>1.94</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>1.85</t>
+          <t>1.91</t>
         </is>
       </c>
       <c r="N34" t="inlineStr"/>
@@ -3147,6 +3251,966 @@
       <c r="U34" t="inlineStr"/>
       <c r="V34" t="inlineStr"/>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Liga Portugal 2 - PRT SL</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Paços de Ferreira vs Farense</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2025-12-28 14:00:00</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>3.50</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>3.25</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>1.95</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>3.62</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>3.37</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>2.07</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>1.83</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>1.83</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
+      <c r="N35" t="inlineStr"/>
+      <c r="O35" t="inlineStr"/>
+      <c r="P35" t="inlineStr"/>
+      <c r="Q35" t="inlineStr"/>
+      <c r="R35" t="inlineStr"/>
+      <c r="S35" t="inlineStr"/>
+      <c r="T35" t="inlineStr"/>
+      <c r="U35" t="inlineStr"/>
+      <c r="V35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Liga Portugal - PRT PL</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Casa Pia vs Vitória Guimarães</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2025-12-28 15:30:00</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>3.30</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2.30</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>3.41</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>3.07</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>2.32</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>1.70</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>2.05</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>1.74</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>2.10</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr"/>
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr"/>
+      <c r="Q36" t="inlineStr"/>
+      <c r="R36" t="inlineStr"/>
+      <c r="S36" t="inlineStr"/>
+      <c r="T36" t="inlineStr"/>
+      <c r="U36" t="inlineStr"/>
+      <c r="V36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Liga Portugal - PRT PL</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Arouca vs Gil Vicente</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2025-12-28 15:30:00</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>4.00</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>3.20</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>1.95</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>4.09</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>3.36</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>1.96</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>1.80</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>1.95</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>1.82</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr"/>
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr"/>
+      <c r="Q37" t="inlineStr"/>
+      <c r="R37" t="inlineStr"/>
+      <c r="S37" t="inlineStr"/>
+      <c r="T37" t="inlineStr"/>
+      <c r="U37" t="inlineStr"/>
+      <c r="V37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Premier League - UK PL</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Crystal Palace vs Tottenham Hotspur</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2025-12-28 16:30:00</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>3.25</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>3.20</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>2.32</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>3.28</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>3.37</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>2.09</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>1.79</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr"/>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>1.85</t>
+        </is>
+      </c>
+      <c r="Q38" t="inlineStr"/>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>2.05</t>
+        </is>
+      </c>
+      <c r="S38" t="inlineStr"/>
+      <c r="T38" t="inlineStr">
+        <is>
+          <t>1.84</t>
+        </is>
+      </c>
+      <c r="U38" t="inlineStr"/>
+      <c r="V38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Serie A - ITA SA</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Bologna vs Sassuolo</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2025-12-28 17:00:00</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>1.70</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>3.70</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>4.75</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>1.71</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>3.83</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>5.21</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>1.80</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>1.95</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>1.93</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>1.92</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr"/>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>1.85</t>
+        </is>
+      </c>
+      <c r="Q39" t="inlineStr"/>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>2.02</t>
+        </is>
+      </c>
+      <c r="S39" t="inlineStr"/>
+      <c r="T39" t="inlineStr">
+        <is>
+          <t>1.87</t>
+        </is>
+      </c>
+      <c r="U39" t="inlineStr"/>
+      <c r="V39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Liga Portugal - PRT PL</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Sporting Braga vs Benfica</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2025-12-28 18:00:00</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>3.30</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>3.30</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>2.15</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>3.42</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>3.31</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>2.19</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>1.95</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>1.80</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>1.95</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>1.85</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>1.80</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>2.05</t>
+        </is>
+      </c>
+      <c r="Q40" t="inlineStr"/>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>2.05</t>
+        </is>
+      </c>
+      <c r="S40" t="inlineStr"/>
+      <c r="T40" t="inlineStr">
+        <is>
+          <t>1.80</t>
+        </is>
+      </c>
+      <c r="U40" t="inlineStr"/>
+      <c r="V40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Serie A - ITA SA</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Atalanta vs Inter</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2025-12-28 19:45:00</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>3.50</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>3.50</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>3.66</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>3.66</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>2.05</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>2.20</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>1.61</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>2.32</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>1.64</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>1.85</t>
+        </is>
+      </c>
+      <c r="Q41" t="inlineStr"/>
+      <c r="R41" t="inlineStr"/>
+      <c r="S41" t="inlineStr"/>
+      <c r="T41" t="inlineStr"/>
+      <c r="U41" t="inlineStr"/>
+      <c r="V41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Liga Portugal - PRT PL</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Sporting CP vs Rio Ave</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2025-12-28 20:30:00</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>1.14</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>7.00</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>17.00</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>1.14</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>8.95</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>15.32</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>1.70</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>2.05</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>1.66</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>2.21</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr"/>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
+      <c r="P42" t="inlineStr"/>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>1.85</t>
+        </is>
+      </c>
+      <c r="R42" t="inlineStr"/>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="T42" t="inlineStr"/>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>1.83</t>
+        </is>
+      </c>
+      <c r="V42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Pro League - SAU PL</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Al Khaleej vs Al Fateh</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2025-12-29 14:35:00</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
+      <c r="N43" t="inlineStr"/>
+      <c r="O43" t="inlineStr"/>
+      <c r="P43" t="inlineStr"/>
+      <c r="Q43" t="inlineStr"/>
+      <c r="R43" t="inlineStr"/>
+      <c r="S43" t="inlineStr"/>
+      <c r="T43" t="inlineStr"/>
+      <c r="U43" t="inlineStr"/>
+      <c r="V43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Pro League - SAU PL</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Al Taawoun vs Al Najma</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2025-12-29 17:30:00</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr"/>
+      <c r="O44" t="inlineStr"/>
+      <c r="P44" t="inlineStr"/>
+      <c r="Q44" t="inlineStr"/>
+      <c r="R44" t="inlineStr"/>
+      <c r="S44" t="inlineStr"/>
+      <c r="T44" t="inlineStr"/>
+      <c r="U44" t="inlineStr"/>
+      <c r="V44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Pro League - SAU PL</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Al Riyadh vs Al Hazm</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>2025-12-29 17:30:00</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>2.58</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>3.23</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>2.72</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr"/>
+      <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr"/>
+      <c r="Q45" t="inlineStr"/>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>2.03</t>
+        </is>
+      </c>
+      <c r="S45" t="inlineStr"/>
+      <c r="T45" t="inlineStr">
+        <is>
+          <t>1.77</t>
+        </is>
+      </c>
+      <c r="U45" t="inlineStr"/>
+      <c r="V45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Serie A - ITA SA</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Roma vs Genoa</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>2025-12-29 19:45:00</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>1.60</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>3.60</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>6.25</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>1.64</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>3.73</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>6.32</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>1.57</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>1.60</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>2.41</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr"/>
+      <c r="O46" t="inlineStr"/>
+      <c r="P46" t="inlineStr"/>
+      <c r="Q46" t="inlineStr"/>
+      <c r="R46" t="inlineStr"/>
+      <c r="S46" t="inlineStr"/>
+      <c r="T46" t="inlineStr"/>
+      <c r="U46" t="inlineStr"/>
+      <c r="V46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Liga Portugal - PRT PL</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Porto vs AVS</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2025-12-29 20:15:00</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>1.12</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>8.00</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>21.00</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>1.10</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>9.58</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>24.90</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>1.53</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>2.37</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>1.49</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>2.60</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr"/>
+      <c r="O47" t="inlineStr"/>
+      <c r="P47" t="inlineStr"/>
+      <c r="Q47" t="inlineStr"/>
+      <c r="R47" t="inlineStr"/>
+      <c r="S47" t="inlineStr">
+        <is>
+          <t>1.95</t>
+        </is>
+      </c>
+      <c r="T47" t="inlineStr"/>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>1.86</t>
+        </is>
+      </c>
+      <c r="V47" t="inlineStr"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="V2" r:id="rId1"/>

</xml_diff>